<commit_message>
Made an english sql, modified README-file
</commit_message>
<xml_diff>
--- a/online_store_docs/Web-project_resurssit.xlsx
+++ b/online_store_docs/Web-project_resurssit.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_EC33C3647F337B4EDEDCD7DEE3B7B3B82C73F598" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{2A1AAB8C-A72A-4D8A-A402-857B4B283D3C}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leevi\Desktop\K8397\online-store-laravel-react\online_store_docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93440073-D192-4276-B540-1036C79739EE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Pvm.</t>
   </si>
@@ -68,13 +73,16 @@
   </si>
   <si>
     <t>Tietokanta ver1.0 ja dokumentti</t>
+  </si>
+  <si>
+    <t>Tietokanta englanniksi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,7 +124,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -132,7 +140,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-teema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -428,19 +436,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:S5"/>
+  <dimension ref="A2:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -477,7 +485,7 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -497,7 +505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>10</v>
       </c>
@@ -508,7 +516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -520,6 +528,17 @@
       </c>
       <c r="E5">
         <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -528,12 +547,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -683,19 +699,45 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99E4A391-7E8A-442B-B7AA-4A117E9154C6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0885ADCA-5AA5-43A1-AB79-2C157DC25D1E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F09259AD-2121-47F7-925D-5FED5E9F706F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F09259AD-2121-47F7-925D-5FED5E9F706F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2207c59d-12b6-45bf-988a-69ce320217fe"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0885ADCA-5AA5-43A1-AB79-2C157DC25D1E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99E4A391-7E8A-442B-B7AA-4A117E9154C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>